<commit_message>
actualiza notas estudiantes taller 3
</commit_message>
<xml_diff>
--- a/MONITOR/2021-2/Taller3/Estudiantes.xlsx
+++ b/MONITOR/2021-2/Taller3/Estudiantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UJ\UJ2021-01\Monitorias\revisionTrabajos\MONITOR\2021-2\Taller3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A438514-5AED-4464-AAED-80BD25D204D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56AEF5D-4A6B-47F7-BE65-48F4B5AD45D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -198,6 +198,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -382,7 +388,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -446,6 +452,9 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4370,9 +4379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E15" sqref="E15"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -4509,9 +4518,15 @@
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D10" s="6">
+        <v>9</v>
+      </c>
       <c r="E10" s="10"/>
       <c r="F10" s="8"/>
       <c r="G10" s="12"/>
@@ -4522,9 +4537,15 @@
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="14">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14">
+        <v>7</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="8"/>
       <c r="G11" s="12"/>
@@ -4556,9 +4577,15 @@
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="B13" s="6">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6">
+        <v>10</v>
+      </c>
       <c r="E13" s="10"/>
       <c r="F13" s="8"/>
       <c r="G13" s="12"/>
@@ -4633,9 +4660,15 @@
       <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="6">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6">
+        <v>10</v>
+      </c>
       <c r="E18" s="10"/>
       <c r="F18" s="8"/>
       <c r="G18" s="12"/>
@@ -4665,9 +4698,15 @@
       <c r="A20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="B20" s="6">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6">
+        <v>10</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="8"/>
       <c r="G20" s="12"/>

</xml_diff>